<commit_message>
Corrected setup fee from Priska
</commit_message>
<xml_diff>
--- a/WebRoot/costcenter_resources/UWPR_Current_Rates.xlsx
+++ b/WebRoot/costcenter_resources/UWPR_Current_Rates.xlsx
@@ -1651,16 +1651,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="14" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3992,11 +3992,11 @@
       <c r="B11" s="11"/>
       <c r="C11" s="9"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="203"/>
-      <c r="F11" s="203"/>
-      <c r="G11" s="203"/>
-      <c r="H11" s="203"/>
-      <c r="I11" s="203"/>
+      <c r="E11" s="206"/>
+      <c r="F11" s="206"/>
+      <c r="G11" s="206"/>
+      <c r="H11" s="206"/>
+      <c r="I11" s="206"/>
       <c r="M11" s="13" t="s">
         <v>12</v>
       </c>
@@ -4004,21 +4004,21 @@
     <row r="12" spans="2:21" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C12" s="9"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="203"/>
-      <c r="F12" s="203"/>
-      <c r="G12" s="203"/>
-      <c r="H12" s="203"/>
-      <c r="I12" s="203"/>
+      <c r="E12" s="206"/>
+      <c r="F12" s="206"/>
+      <c r="G12" s="206"/>
+      <c r="H12" s="206"/>
+      <c r="I12" s="206"/>
       <c r="M12" s="14"/>
     </row>
     <row r="13" spans="2:21" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C13" s="9"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="203"/>
-      <c r="F13" s="203"/>
-      <c r="G13" s="203"/>
-      <c r="H13" s="203"/>
-      <c r="I13" s="203"/>
+      <c r="E13" s="206"/>
+      <c r="F13" s="206"/>
+      <c r="G13" s="206"/>
+      <c r="H13" s="206"/>
+      <c r="I13" s="206"/>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
@@ -4477,36 +4477,36 @@
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="56"/>
-      <c r="B33" s="204" t="s">
+      <c r="B33" s="205" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="204"/>
-      <c r="D33" s="204"/>
-      <c r="E33" s="205">
+      <c r="C33" s="205"/>
+      <c r="D33" s="205"/>
+      <c r="E33" s="203">
         <f>(E31/100)*10</f>
         <v>3.7</v>
       </c>
-      <c r="F33" s="205">
+      <c r="F33" s="203">
         <f>(F31/100)*10</f>
         <v>3.3000000000000003</v>
       </c>
-      <c r="G33" s="205">
+      <c r="G33" s="203">
         <f t="shared" ref="G33:K33" si="3">(G31/100)*10</f>
         <v>3.3000000000000003</v>
       </c>
-      <c r="H33" s="205">
+      <c r="H33" s="203">
         <f t="shared" si="3"/>
         <v>3.625</v>
       </c>
-      <c r="I33" s="205">
+      <c r="I33" s="203">
         <f t="shared" si="3"/>
         <v>3.85</v>
       </c>
-      <c r="J33" s="205">
+      <c r="J33" s="203">
         <f t="shared" si="3"/>
         <v>3.85</v>
       </c>
-      <c r="K33" s="205">
+      <c r="K33" s="203">
         <f t="shared" si="3"/>
         <v>3.85</v>
       </c>
@@ -4515,51 +4515,51 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="56"/>
-      <c r="B34" s="204"/>
-      <c r="C34" s="204"/>
-      <c r="D34" s="204"/>
-      <c r="E34" s="205"/>
-      <c r="F34" s="205"/>
-      <c r="G34" s="205"/>
-      <c r="H34" s="205"/>
-      <c r="I34" s="205"/>
-      <c r="J34" s="205"/>
-      <c r="K34" s="205"/>
+      <c r="B34" s="205"/>
+      <c r="C34" s="205"/>
+      <c r="D34" s="205"/>
+      <c r="E34" s="203"/>
+      <c r="F34" s="203"/>
+      <c r="G34" s="203"/>
+      <c r="H34" s="203"/>
+      <c r="I34" s="203"/>
+      <c r="J34" s="203"/>
+      <c r="K34" s="203"/>
       <c r="L34" s="56"/>
       <c r="M34" s="5"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="56"/>
-      <c r="B35" s="204" t="s">
+      <c r="B35" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="204"/>
-      <c r="D35" s="204"/>
-      <c r="E35" s="205">
+      <c r="C35" s="205"/>
+      <c r="D35" s="205"/>
+      <c r="E35" s="203">
         <f>(E31/100)*90</f>
         <v>33.299999999999997</v>
       </c>
-      <c r="F35" s="205">
+      <c r="F35" s="203">
         <f t="shared" ref="F35:K35" si="4">(F31/100)*90</f>
         <v>29.700000000000003</v>
       </c>
-      <c r="G35" s="205">
+      <c r="G35" s="203">
         <f t="shared" si="4"/>
         <v>29.700000000000003</v>
       </c>
-      <c r="H35" s="205">
+      <c r="H35" s="203">
         <f t="shared" si="4"/>
         <v>32.625</v>
       </c>
-      <c r="I35" s="205">
+      <c r="I35" s="203">
         <f t="shared" si="4"/>
         <v>34.65</v>
       </c>
-      <c r="J35" s="205">
+      <c r="J35" s="203">
         <f t="shared" si="4"/>
         <v>34.65</v>
       </c>
-      <c r="K35" s="205">
+      <c r="K35" s="203">
         <f t="shared" si="4"/>
         <v>34.65</v>
       </c>
@@ -4568,16 +4568,16 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="56"/>
-      <c r="B36" s="204"/>
-      <c r="C36" s="204"/>
-      <c r="D36" s="204"/>
-      <c r="E36" s="205"/>
-      <c r="F36" s="205"/>
-      <c r="G36" s="205"/>
-      <c r="H36" s="205"/>
-      <c r="I36" s="205"/>
-      <c r="J36" s="205"/>
-      <c r="K36" s="205"/>
+      <c r="B36" s="205"/>
+      <c r="C36" s="205"/>
+      <c r="D36" s="205"/>
+      <c r="E36" s="203"/>
+      <c r="F36" s="203"/>
+      <c r="G36" s="203"/>
+      <c r="H36" s="203"/>
+      <c r="I36" s="203"/>
+      <c r="J36" s="203"/>
+      <c r="K36" s="203"/>
       <c r="L36" s="56"/>
       <c r="M36" s="5"/>
     </row>
@@ -5147,101 +5147,101 @@
       <c r="M62" s="5"/>
     </row>
     <row r="63" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="204" t="s">
+      <c r="B63" s="205" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="204"/>
-      <c r="D63" s="204"/>
-      <c r="E63" s="205">
+      <c r="C63" s="205"/>
+      <c r="D63" s="205"/>
+      <c r="E63" s="203">
         <f>(E61/100)*10</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="F63" s="205">
+      <c r="F63" s="203">
         <f t="shared" ref="F63:K63" si="10">(F61/100)*10</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="G63" s="205">
+      <c r="G63" s="203">
         <f t="shared" si="10"/>
         <v>4.0999999999999996</v>
       </c>
-      <c r="H63" s="205">
+      <c r="H63" s="203">
         <f t="shared" si="10"/>
         <v>4.75</v>
       </c>
-      <c r="I63" s="205">
+      <c r="I63" s="203">
         <f t="shared" si="10"/>
         <v>5.2</v>
       </c>
-      <c r="J63" s="205">
+      <c r="J63" s="203">
         <f t="shared" si="10"/>
         <v>5.2</v>
       </c>
-      <c r="K63" s="205">
+      <c r="K63" s="203">
         <f t="shared" si="10"/>
         <v>5.2</v>
       </c>
       <c r="M63" s="5"/>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B64" s="204"/>
-      <c r="C64" s="204"/>
-      <c r="D64" s="204"/>
-      <c r="E64" s="205"/>
-      <c r="F64" s="205"/>
-      <c r="G64" s="205"/>
-      <c r="H64" s="205"/>
-      <c r="I64" s="205"/>
-      <c r="J64" s="205"/>
-      <c r="K64" s="205"/>
+      <c r="B64" s="205"/>
+      <c r="C64" s="205"/>
+      <c r="D64" s="205"/>
+      <c r="E64" s="203"/>
+      <c r="F64" s="203"/>
+      <c r="G64" s="203"/>
+      <c r="H64" s="203"/>
+      <c r="I64" s="203"/>
+      <c r="J64" s="203"/>
+      <c r="K64" s="203"/>
       <c r="M64" s="5"/>
     </row>
     <row r="65" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="204" t="s">
+      <c r="B65" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="C65" s="204"/>
-      <c r="D65" s="204"/>
-      <c r="E65" s="205">
+      <c r="C65" s="205"/>
+      <c r="D65" s="205"/>
+      <c r="E65" s="203">
         <f>(E61/100)*90</f>
         <v>44.1</v>
       </c>
-      <c r="F65" s="205">
+      <c r="F65" s="203">
         <f t="shared" ref="F65:K65" si="11">(F61/100)*90</f>
         <v>36.9</v>
       </c>
-      <c r="G65" s="205">
+      <c r="G65" s="203">
         <f t="shared" si="11"/>
         <v>36.9</v>
       </c>
-      <c r="H65" s="205">
+      <c r="H65" s="203">
         <f t="shared" si="11"/>
         <v>42.75</v>
       </c>
-      <c r="I65" s="205">
+      <c r="I65" s="203">
         <f t="shared" si="11"/>
         <v>46.800000000000004</v>
       </c>
-      <c r="J65" s="205">
+      <c r="J65" s="203">
         <f t="shared" si="11"/>
         <v>46.800000000000004</v>
       </c>
-      <c r="K65" s="205">
+      <c r="K65" s="203">
         <f t="shared" si="11"/>
         <v>46.800000000000004</v>
       </c>
       <c r="M65" s="5"/>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="204"/>
-      <c r="C66" s="204"/>
-      <c r="D66" s="204"/>
-      <c r="E66" s="205"/>
-      <c r="F66" s="205"/>
-      <c r="G66" s="205"/>
-      <c r="H66" s="205"/>
-      <c r="I66" s="205"/>
-      <c r="J66" s="205"/>
-      <c r="K66" s="205"/>
+      <c r="B66" s="205"/>
+      <c r="C66" s="205"/>
+      <c r="D66" s="205"/>
+      <c r="E66" s="203"/>
+      <c r="F66" s="203"/>
+      <c r="G66" s="203"/>
+      <c r="H66" s="203"/>
+      <c r="I66" s="203"/>
+      <c r="J66" s="203"/>
+      <c r="K66" s="203"/>
       <c r="M66" s="5"/>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
@@ -5799,101 +5799,101 @@
       <c r="M92" s="5"/>
     </row>
     <row r="93" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="206" t="s">
+      <c r="B93" s="204" t="s">
         <v>40</v>
       </c>
-      <c r="C93" s="206"/>
-      <c r="D93" s="206"/>
-      <c r="E93" s="205">
+      <c r="C93" s="204"/>
+      <c r="D93" s="204"/>
+      <c r="E93" s="203">
         <f>(E91/100)*10</f>
         <v>10.725999999999999</v>
       </c>
-      <c r="F93" s="205">
+      <c r="F93" s="203">
         <f t="shared" ref="F93:K93" si="17">(F91/100)*10</f>
         <v>11.261000000000001</v>
       </c>
-      <c r="G93" s="205">
+      <c r="G93" s="203">
         <f t="shared" si="17"/>
         <v>10.725999999999999</v>
       </c>
-      <c r="H93" s="205">
+      <c r="H93" s="203">
         <f t="shared" si="17"/>
         <v>13.25</v>
       </c>
-      <c r="I93" s="205">
+      <c r="I93" s="203">
         <f t="shared" si="17"/>
         <v>10.837000000000002</v>
       </c>
-      <c r="J93" s="205">
+      <c r="J93" s="203">
         <f t="shared" si="17"/>
         <v>11.585000000000001</v>
       </c>
-      <c r="K93" s="205">
+      <c r="K93" s="203">
         <f t="shared" si="17"/>
         <v>11.585000000000001</v>
       </c>
       <c r="M93" s="5"/>
     </row>
     <row r="94" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B94" s="206"/>
-      <c r="C94" s="206"/>
-      <c r="D94" s="206"/>
-      <c r="E94" s="205"/>
-      <c r="F94" s="205"/>
-      <c r="G94" s="205"/>
-      <c r="H94" s="205"/>
-      <c r="I94" s="205"/>
-      <c r="J94" s="205"/>
-      <c r="K94" s="205"/>
+      <c r="B94" s="204"/>
+      <c r="C94" s="204"/>
+      <c r="D94" s="204"/>
+      <c r="E94" s="203"/>
+      <c r="F94" s="203"/>
+      <c r="G94" s="203"/>
+      <c r="H94" s="203"/>
+      <c r="I94" s="203"/>
+      <c r="J94" s="203"/>
+      <c r="K94" s="203"/>
       <c r="M94" s="5"/>
     </row>
     <row r="95" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="206" t="s">
+      <c r="B95" s="204" t="s">
         <v>41</v>
       </c>
-      <c r="C95" s="206"/>
-      <c r="D95" s="206"/>
-      <c r="E95" s="205">
+      <c r="C95" s="204"/>
+      <c r="D95" s="204"/>
+      <c r="E95" s="203">
         <f>(E91/100)*90</f>
         <v>96.534000000000006</v>
       </c>
-      <c r="F95" s="205">
+      <c r="F95" s="203">
         <f t="shared" ref="F95:K95" si="18">(F91/100)*90</f>
         <v>101.349</v>
       </c>
-      <c r="G95" s="205">
+      <c r="G95" s="203">
         <f t="shared" si="18"/>
         <v>96.534000000000006</v>
       </c>
-      <c r="H95" s="205">
+      <c r="H95" s="203">
         <f t="shared" si="18"/>
         <v>119.25</v>
       </c>
-      <c r="I95" s="205">
+      <c r="I95" s="203">
         <f t="shared" si="18"/>
         <v>97.533000000000015</v>
       </c>
-      <c r="J95" s="205">
+      <c r="J95" s="203">
         <f t="shared" si="18"/>
         <v>104.26500000000001</v>
       </c>
-      <c r="K95" s="205">
+      <c r="K95" s="203">
         <f t="shared" si="18"/>
         <v>104.26500000000001</v>
       </c>
       <c r="M95" s="5"/>
     </row>
     <row r="96" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B96" s="206"/>
-      <c r="C96" s="206"/>
-      <c r="D96" s="206"/>
-      <c r="E96" s="205"/>
-      <c r="F96" s="205"/>
-      <c r="G96" s="205"/>
-      <c r="H96" s="205"/>
-      <c r="I96" s="205"/>
-      <c r="J96" s="205"/>
-      <c r="K96" s="205"/>
+      <c r="B96" s="204"/>
+      <c r="C96" s="204"/>
+      <c r="D96" s="204"/>
+      <c r="E96" s="203"/>
+      <c r="F96" s="203"/>
+      <c r="G96" s="203"/>
+      <c r="H96" s="203"/>
+      <c r="I96" s="203"/>
+      <c r="J96" s="203"/>
+      <c r="K96" s="203"/>
       <c r="M96" s="5"/>
     </row>
     <row r="97" spans="2:13" x14ac:dyDescent="0.25">
@@ -6413,103 +6413,103 @@
       <c r="M122" s="5"/>
     </row>
     <row r="123" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="206" t="s">
+      <c r="B123" s="204" t="s">
         <v>40</v>
       </c>
-      <c r="C123" s="206"/>
-      <c r="D123" s="206"/>
-      <c r="E123" s="205">
+      <c r="C123" s="204"/>
+      <c r="D123" s="204"/>
+      <c r="E123" s="203">
         <f>(E121/100)*10</f>
         <v>16.603000000000002</v>
       </c>
-      <c r="F123" s="205">
+      <c r="F123" s="203">
         <f t="shared" ref="F123:K123" si="24">(F121/100)*10</f>
         <v>16.603000000000002</v>
       </c>
-      <c r="G123" s="205">
+      <c r="G123" s="203">
         <f t="shared" si="24"/>
         <v>16.603000000000002</v>
       </c>
-      <c r="H123" s="205">
+      <c r="H123" s="203">
         <f t="shared" si="24"/>
         <v>18.593000000000004</v>
       </c>
-      <c r="I123" s="205">
+      <c r="I123" s="203">
         <f t="shared" si="24"/>
         <v>23.872000000000003</v>
       </c>
-      <c r="J123" s="205">
+      <c r="J123" s="203">
         <f t="shared" si="24"/>
         <v>23.872000000000003</v>
       </c>
-      <c r="K123" s="205">
+      <c r="K123" s="203">
         <f t="shared" si="24"/>
         <v>23.872000000000003</v>
       </c>
       <c r="M123" s="5"/>
     </row>
     <row r="124" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B124" s="206"/>
-      <c r="C124" s="206"/>
-      <c r="D124" s="206"/>
-      <c r="E124" s="205"/>
-      <c r="F124" s="205"/>
-      <c r="G124" s="205"/>
-      <c r="H124" s="205"/>
-      <c r="I124" s="205"/>
-      <c r="J124" s="205"/>
-      <c r="K124" s="205"/>
+      <c r="B124" s="204"/>
+      <c r="C124" s="204"/>
+      <c r="D124" s="204"/>
+      <c r="E124" s="203"/>
+      <c r="F124" s="203"/>
+      <c r="G124" s="203"/>
+      <c r="H124" s="203"/>
+      <c r="I124" s="203"/>
+      <c r="J124" s="203"/>
+      <c r="K124" s="203"/>
       <c r="L124" s="7"/>
       <c r="M124" s="5"/>
       <c r="U124" s="106"/>
     </row>
     <row r="125" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="206" t="s">
+      <c r="B125" s="204" t="s">
         <v>41</v>
       </c>
-      <c r="C125" s="206"/>
-      <c r="D125" s="206"/>
-      <c r="E125" s="205">
+      <c r="C125" s="204"/>
+      <c r="D125" s="204"/>
+      <c r="E125" s="203">
         <f>(E121/100)*90</f>
         <v>149.42700000000002</v>
       </c>
-      <c r="F125" s="205">
+      <c r="F125" s="203">
         <f t="shared" ref="F125:K125" si="25">(F121/100)*90</f>
         <v>149.42700000000002</v>
       </c>
-      <c r="G125" s="205">
+      <c r="G125" s="203">
         <f t="shared" si="25"/>
         <v>149.42700000000002</v>
       </c>
-      <c r="H125" s="205">
+      <c r="H125" s="203">
         <f t="shared" si="25"/>
         <v>167.33700000000002</v>
       </c>
-      <c r="I125" s="205">
+      <c r="I125" s="203">
         <f t="shared" si="25"/>
         <v>214.84800000000004</v>
       </c>
-      <c r="J125" s="205">
+      <c r="J125" s="203">
         <f t="shared" si="25"/>
         <v>214.84800000000004</v>
       </c>
-      <c r="K125" s="205">
+      <c r="K125" s="203">
         <f t="shared" si="25"/>
         <v>214.84800000000004</v>
       </c>
       <c r="M125" s="5"/>
     </row>
     <row r="126" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B126" s="206"/>
-      <c r="C126" s="206"/>
-      <c r="D126" s="206"/>
-      <c r="E126" s="205"/>
-      <c r="F126" s="205"/>
-      <c r="G126" s="205"/>
-      <c r="H126" s="205"/>
-      <c r="I126" s="205"/>
-      <c r="J126" s="205"/>
-      <c r="K126" s="205"/>
+      <c r="B126" s="204"/>
+      <c r="C126" s="204"/>
+      <c r="D126" s="204"/>
+      <c r="E126" s="203"/>
+      <c r="F126" s="203"/>
+      <c r="G126" s="203"/>
+      <c r="H126" s="203"/>
+      <c r="I126" s="203"/>
+      <c r="J126" s="203"/>
+      <c r="K126" s="203"/>
       <c r="M126" s="5"/>
     </row>
     <row r="127" spans="2:21" x14ac:dyDescent="0.25">
@@ -6539,6 +6539,57 @@
     <protectedRange sqref="D27 D57 D87 D117" name="Range1"/>
   </protectedRanges>
   <mergeCells count="67">
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="B33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="B35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="J63:J64"/>
+    <mergeCell ref="K63:K64"/>
+    <mergeCell ref="B65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="I65:I66"/>
+    <mergeCell ref="J65:J66"/>
+    <mergeCell ref="K65:K66"/>
+    <mergeCell ref="B63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="I63:I64"/>
+    <mergeCell ref="J93:J94"/>
+    <mergeCell ref="K93:K94"/>
+    <mergeCell ref="B95:D96"/>
+    <mergeCell ref="E95:E96"/>
+    <mergeCell ref="F95:F96"/>
+    <mergeCell ref="G95:G96"/>
+    <mergeCell ref="H95:H96"/>
+    <mergeCell ref="I95:I96"/>
+    <mergeCell ref="J95:J96"/>
+    <mergeCell ref="K95:K96"/>
+    <mergeCell ref="B93:D94"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="G93:G94"/>
+    <mergeCell ref="H93:H94"/>
+    <mergeCell ref="I93:I94"/>
     <mergeCell ref="J123:J124"/>
     <mergeCell ref="K123:K124"/>
     <mergeCell ref="B125:D126"/>
@@ -6555,57 +6606,6 @@
     <mergeCell ref="G123:G124"/>
     <mergeCell ref="H123:H124"/>
     <mergeCell ref="I123:I124"/>
-    <mergeCell ref="J93:J94"/>
-    <mergeCell ref="K93:K94"/>
-    <mergeCell ref="B95:D96"/>
-    <mergeCell ref="E95:E96"/>
-    <mergeCell ref="F95:F96"/>
-    <mergeCell ref="G95:G96"/>
-    <mergeCell ref="H95:H96"/>
-    <mergeCell ref="I95:I96"/>
-    <mergeCell ref="J95:J96"/>
-    <mergeCell ref="K95:K96"/>
-    <mergeCell ref="B93:D94"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="G93:G94"/>
-    <mergeCell ref="H93:H94"/>
-    <mergeCell ref="I93:I94"/>
-    <mergeCell ref="J63:J64"/>
-    <mergeCell ref="K63:K64"/>
-    <mergeCell ref="B65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="I65:I66"/>
-    <mergeCell ref="J65:J66"/>
-    <mergeCell ref="K65:K66"/>
-    <mergeCell ref="B63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="I63:I64"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="B35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="B33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M11" r:id="rId1"/>
@@ -6658,7 +6658,7 @@
         <v>46</v>
       </c>
       <c r="I1" s="109">
-        <v>43411</v>
+        <v>43665</v>
       </c>
       <c r="AH1" s="4"/>
       <c r="AI1" s="4"/>
@@ -8072,29 +8072,29 @@
         <v>24</v>
       </c>
       <c r="D41" s="195">
-        <f>'20181101'!E$50</f>
-        <v>24</v>
+        <f>'20181101'!E60</f>
+        <v>25</v>
       </c>
       <c r="E41" s="196"/>
       <c r="F41" s="197">
         <f t="shared" ref="F41:G43" si="5">F$24*$C41+$D41</f>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G41" s="198">
         <f t="shared" si="5"/>
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H41" s="197">
         <f t="shared" ref="H41:J47" si="6">H$24*$C41+$D41</f>
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I41" s="197">
         <f t="shared" si="6"/>
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J41" s="197">
         <f t="shared" si="6"/>
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K41" s="110"/>
       <c r="L41" s="183"/>
@@ -8117,29 +8117,29 @@
         <v>16</v>
       </c>
       <c r="D42" s="195">
-        <f>'20181101'!F$50</f>
-        <v>16</v>
+        <f>'20181101'!F60</f>
+        <v>25</v>
       </c>
       <c r="E42" s="196"/>
       <c r="F42" s="197">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G42" s="198">
         <f t="shared" si="5"/>
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="H42" s="197">
         <f t="shared" si="6"/>
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="I42" s="197">
         <f t="shared" si="6"/>
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="J42" s="197">
         <f t="shared" si="6"/>
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="K42" s="110"/>
       <c r="L42" s="110"/>
@@ -8162,29 +8162,29 @@
         <v>16</v>
       </c>
       <c r="D43" s="195">
-        <f>'20181101'!G$50</f>
-        <v>16</v>
+        <f>'20181101'!G60</f>
+        <v>25</v>
       </c>
       <c r="E43" s="196"/>
       <c r="F43" s="197">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G43" s="198">
         <f t="shared" si="5"/>
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="H43" s="197">
         <f>H$24*$C43+$D43</f>
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="I43" s="197">
         <f>I$24*$C43+$D43</f>
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="J43" s="197">
         <f t="shared" si="6"/>
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="K43" s="110"/>
       <c r="L43" s="110"/>
@@ -8207,29 +8207,29 @@
         <v>22.5</v>
       </c>
       <c r="D44" s="195">
-        <f>'20181101'!H$50</f>
-        <v>22.5</v>
+        <f>'20181101'!H60</f>
+        <v>25</v>
       </c>
       <c r="E44" s="196"/>
       <c r="F44" s="197">
         <f>F$24*$C44+$D44</f>
-        <v>112.5</v>
+        <v>115</v>
       </c>
       <c r="G44" s="198">
         <f t="shared" ref="F44:G47" si="7">G$24*$C44+$D44</f>
-        <v>135</v>
+        <v>137.5</v>
       </c>
       <c r="H44" s="197">
         <f>H$24*$C44+$D44</f>
-        <v>135</v>
+        <v>137.5</v>
       </c>
       <c r="I44" s="197">
         <f>I$24*$C44+$D44</f>
-        <v>157.5</v>
+        <v>160</v>
       </c>
       <c r="J44" s="197">
         <f>J$24*$C44+$D44</f>
-        <v>157.5</v>
+        <v>160</v>
       </c>
       <c r="K44" s="110"/>
       <c r="L44" s="110"/>
@@ -8248,29 +8248,29 @@
         <v>27</v>
       </c>
       <c r="D45" s="195">
-        <f>'20181101'!I$50</f>
-        <v>27</v>
+        <f>'20181101'!I60</f>
+        <v>25</v>
       </c>
       <c r="E45" s="196"/>
       <c r="F45" s="197">
         <f t="shared" si="7"/>
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G45" s="198">
         <f t="shared" si="7"/>
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H45" s="197">
         <f t="shared" si="6"/>
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I45" s="197">
         <f t="shared" si="6"/>
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J45" s="197">
         <f>J$24*$C45+$D45</f>
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K45" s="110"/>
       <c r="L45" s="110"/>
@@ -8293,29 +8293,29 @@
         <v>27</v>
       </c>
       <c r="D46" s="195">
-        <f>'20181101'!J$50</f>
-        <v>27</v>
+        <f>'20181101'!J60</f>
+        <v>25</v>
       </c>
       <c r="E46" s="199"/>
       <c r="F46" s="197">
         <f t="shared" si="7"/>
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G46" s="198">
         <f t="shared" si="7"/>
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H46" s="197">
         <f t="shared" si="6"/>
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I46" s="197">
         <f t="shared" si="6"/>
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J46" s="197">
         <f t="shared" si="6"/>
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K46" s="110"/>
       <c r="L46" s="110"/>
@@ -8338,29 +8338,29 @@
         <v>27</v>
       </c>
       <c r="D47" s="195">
-        <f>'20181101'!K$50</f>
-        <v>27</v>
+        <f>'20181101'!K60</f>
+        <v>25</v>
       </c>
       <c r="E47" s="199"/>
       <c r="F47" s="197">
         <f t="shared" si="7"/>
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G47" s="198">
         <f t="shared" si="7"/>
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H47" s="197">
         <f t="shared" si="6"/>
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I47" s="197">
         <f t="shared" si="6"/>
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J47" s="197">
         <f t="shared" si="6"/>
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K47" s="110"/>
       <c r="N47" s="110"/>

</xml_diff>

<commit_message>
Updates rates and sample submission form.
</commit_message>
<xml_diff>
--- a/WebRoot/costcenter_resources/UWPR_Current_Rates.xlsx
+++ b/WebRoot/costcenter_resources/UWPR_Current_Rates.xlsx
@@ -1,43 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Priska's Stuff\UWPR costcenter\UWPR_Rates\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PriskaStuff\UWPR costcenter\UWPR_Rates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCF6718-1A2C-405F-B46B-650E295B662A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17325"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="20221101 year 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rates 2025_2026" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="In_Out_Both_No">'[1]Selection Options'!$A$15:$A$18</definedName>
+    <definedName name="rates">[2]Analysis!$I$6:$K$10</definedName>
     <definedName name="Yes_No">'[1]Selection Options'!$A$4:$A$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
-  <si>
-    <t>Rates effective 11/1/2022 subject to change without notice</t>
-  </si>
-  <si>
-    <t>revised 11/1/2022</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Instrumentation:</t>
   </si>
@@ -57,22 +65,10 @@
     <t>Orbitrap Fusion</t>
   </si>
   <si>
-    <t>QE+</t>
-  </si>
-  <si>
-    <t>Q Exactive plus</t>
-  </si>
-  <si>
     <t>TSQA</t>
   </si>
   <si>
     <t>TSQ Altis</t>
-  </si>
-  <si>
-    <t>TSQV</t>
-  </si>
-  <si>
-    <t>TSQ Vantage</t>
   </si>
   <si>
     <t>for a detailed description check out our resources webpage</t>
@@ -85,9 +81,6 @@
   </si>
   <si>
     <t>Exploris 2</t>
-  </si>
-  <si>
-    <t>QE +</t>
   </si>
   <si>
     <t>Hourly Rate</t>
@@ -113,17 +106,50 @@
   <si>
     <t>Exploris2</t>
   </si>
+  <si>
+    <t>Astral</t>
+  </si>
+  <si>
+    <t>Orbitrap Astral</t>
+  </si>
+  <si>
+    <t>Enter the number of samples:</t>
+  </si>
+  <si>
+    <t>Number of replicate LC-MS analyses per sample:</t>
+  </si>
+  <si>
+    <t>Number of blanks:</t>
+  </si>
+  <si>
+    <t>Number of extra QC (standards):</t>
+  </si>
+  <si>
+    <t>hrs</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Rates effective 9/1/2024 subject to change without notice</t>
+  </si>
+  <si>
+    <t>Total Estimated Cost:</t>
+  </si>
+  <si>
+    <t>revised 9/1/2025</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +266,21 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -273,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -317,15 +358,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -455,12 +487,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -474,133 +510,83 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="8" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="37" fontId="12" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="37" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="37" fontId="13" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="13" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="37" fontId="13" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="13" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="37" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -613,26 +599,12 @@
     <xf numFmtId="4" fontId="11" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="17" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="17" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="17" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="17" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -641,14 +613,92 @@
     <xf numFmtId="44" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="17" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="12" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="15" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="18" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="37" fontId="12" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink 4" xfId="3" xr:uid="{E0E1D623-BD03-40D9-BD0A-F0EE0A9DF2D5}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -676,7 +726,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -837,7 +887,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="333375" y="352425"/>
-          <a:ext cx="2252327" cy="1471142"/>
+          <a:ext cx="2252327" cy="1461617"/>
           <a:chOff x="4591734" y="1323376"/>
           <a:chExt cx="2252327" cy="1471142"/>
         </a:xfrm>
@@ -2405,7 +2455,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Center - General"/>
@@ -2459,6 +2509,107 @@
         </row>
       </sheetData>
       <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Instructions and Guidance"/>
+      <sheetName val="General Information"/>
+      <sheetName val="Center - Space"/>
+      <sheetName val="Usage"/>
+      <sheetName val="Salaries"/>
+      <sheetName val="Depreciation"/>
+      <sheetName val="Other Costs"/>
+      <sheetName val="Biennium Summary"/>
+      <sheetName val="Add'l Costs"/>
+      <sheetName val="Variance Analysis Report"/>
+      <sheetName val="Approval email"/>
+      <sheetName val="20181101"/>
+      <sheetName val="Analysis"/>
+      <sheetName val="Billings 02.01.17-11.30.17"/>
+      <sheetName val="UWPR rates"/>
+      <sheetName val="20180201"/>
+      <sheetName val="20190201"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12">
+        <row r="6">
+          <cell r="I6" t="str">
+            <v>Fusion</v>
+          </cell>
+          <cell r="J6">
+            <v>13.5</v>
+          </cell>
+          <cell r="K6">
+            <v>27</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="I7" t="str">
+            <v>LTQ-Orbitrap-1</v>
+          </cell>
+          <cell r="J7">
+            <v>8</v>
+          </cell>
+          <cell r="K7">
+            <v>16</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="I8" t="str">
+            <v>Lumos</v>
+          </cell>
+          <cell r="J8">
+            <v>13.5</v>
+          </cell>
+          <cell r="K8">
+            <v>27</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="I9" t="str">
+            <v>Q</v>
+          </cell>
+          <cell r="J9">
+            <v>13.5</v>
+          </cell>
+          <cell r="K9">
+            <v>27</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="I10" t="str">
+            <v>TSQ-Vantage</v>
+          </cell>
+          <cell r="J10">
+            <v>8</v>
+          </cell>
+          <cell r="K10">
+            <v>16</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2726,12 +2877,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:V48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane xSplit="15" ySplit="26" topLeftCell="P27" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P1" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2747,82 +2900,76 @@
     <col min="23" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
+    </row>
+    <row r="2" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="4" t="s">
+    </row>
+    <row r="4" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J5" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J4" s="5" t="s">
+    <row r="6" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J5" s="5" t="s">
+    <row r="7" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J6" s="5" t="s">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="J8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="2" t="s">
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="O10" s="7"/>
+    </row>
+    <row r="12" spans="2:22" ht="18" x14ac:dyDescent="0.25">
+      <c r="C12" s="8" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="J10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" s="7"/>
-    </row>
-    <row r="12" spans="2:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="C12" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
@@ -2830,8 +2977,8 @@
       <c r="G12" s="11"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="14"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="P12" s="14"/>
@@ -2841,908 +2988,883 @@
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
-      <c r="W12" s="15"/>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="15"/>
       <c r="M13" s="14"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="20"/>
-      <c r="U13" s="20"/>
-      <c r="V13" s="20"/>
-      <c r="W13" s="15"/>
-    </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24" t="s">
+      <c r="N13" s="15"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="G14" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" s="15"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="D15" s="82"/>
+      <c r="E15" s="20">
+        <v>17</v>
+      </c>
+      <c r="F15" s="20">
+        <v>17</v>
+      </c>
+      <c r="G15" s="20">
+        <v>17</v>
+      </c>
+      <c r="H15" s="20">
+        <v>17</v>
+      </c>
+      <c r="I15" s="20">
+        <v>17</v>
+      </c>
+      <c r="J15" s="20">
+        <v>15</v>
+      </c>
+      <c r="M15" s="19"/>
+      <c r="N15" s="83"/>
+      <c r="O15" s="83"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="21"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="19"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+    </row>
+    <row r="17" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+      <c r="C17" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="80">
+        <v>1</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="14"/>
+      <c r="C19" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33">
+        <f t="shared" ref="E19" si="0">$D$17*E15</f>
+        <v>17</v>
+      </c>
+      <c r="F19" s="33">
+        <f>$D$17*F15</f>
+        <v>17</v>
+      </c>
+      <c r="G19" s="33">
+        <f>$D$17*G15</f>
+        <v>17</v>
+      </c>
+      <c r="H19" s="33">
+        <f>$D$17*H15</f>
+        <v>17</v>
+      </c>
+      <c r="I19" s="33">
+        <f>$D$17*I15</f>
+        <v>17</v>
+      </c>
+      <c r="J19" s="33">
+        <f>$D$17*J15</f>
+        <v>15</v>
+      </c>
+      <c r="M19" s="14"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="14"/>
+      <c r="C20" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36">
+        <v>27</v>
+      </c>
+      <c r="F20" s="36">
+        <v>27</v>
+      </c>
+      <c r="G20" s="36">
+        <v>27</v>
+      </c>
+      <c r="H20" s="36">
+        <v>27</v>
+      </c>
+      <c r="I20" s="36">
+        <v>27</v>
+      </c>
+      <c r="J20" s="36">
+        <v>27</v>
+      </c>
+      <c r="M20" s="14"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="21"/>
+    </row>
+    <row r="21" spans="2:22" s="41" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="37"/>
+      <c r="C21" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="D21" s="39"/>
+      <c r="E21" s="40">
+        <f t="shared" ref="E21" si="1">E20+E19</f>
+        <v>44</v>
+      </c>
+      <c r="F21" s="40">
+        <f>F20+F19</f>
+        <v>44</v>
+      </c>
+      <c r="G21" s="40">
+        <f>G20+G19</f>
+        <v>44</v>
+      </c>
+      <c r="H21" s="40">
+        <f>H20+H19</f>
+        <v>44</v>
+      </c>
+      <c r="I21" s="40">
+        <f>I20+I19</f>
+        <v>44</v>
+      </c>
+      <c r="J21" s="40">
+        <f>J20+J19</f>
+        <v>42</v>
+      </c>
+      <c r="M21" s="37"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="44"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="44"/>
+      <c r="U21" s="44"/>
+      <c r="V21" s="44"/>
+    </row>
+    <row r="22" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+      <c r="T22" s="45"/>
+      <c r="U22" s="45"/>
+      <c r="V22" s="45"/>
+    </row>
+    <row r="23" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="47"/>
+      <c r="Q23" s="47"/>
+      <c r="R23" s="47"/>
+      <c r="S23" s="47"/>
+      <c r="T23" s="47"/>
+      <c r="U23" s="47"/>
+      <c r="V23" s="47"/>
+    </row>
+    <row r="24" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="47"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="47"/>
+      <c r="T24" s="47"/>
+      <c r="U24" s="47"/>
+      <c r="V24" s="47"/>
+    </row>
+    <row r="25" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="47"/>
+      <c r="Q25" s="47"/>
+      <c r="R25" s="47"/>
+      <c r="S25" s="47"/>
+      <c r="T25" s="47"/>
+      <c r="U25" s="47"/>
+      <c r="V25" s="47"/>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+    </row>
+    <row r="28" spans="2:22" ht="18" x14ac:dyDescent="0.25">
+      <c r="C28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="D28" s="49"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="51"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="48"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="48"/>
+      <c r="T28" s="48"/>
+      <c r="U28" s="48"/>
+      <c r="V28" s="48"/>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="14"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
+      <c r="J29" s="64"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="54"/>
+      <c r="S29" s="54"/>
+      <c r="T29" s="54"/>
+      <c r="U29" s="54"/>
+      <c r="V29" s="54"/>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="22"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="24" t="s">
+      <c r="G30" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="M14" s="20"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
-      <c r="V14" s="26"/>
-      <c r="W14" s="15"/>
-    </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
-      <c r="C15" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30">
-        <v>13.5</v>
-      </c>
-      <c r="F15" s="30">
-        <v>9</v>
-      </c>
-      <c r="G15" s="30">
-        <v>15.5</v>
-      </c>
-      <c r="H15" s="30">
-        <v>15.5</v>
-      </c>
-      <c r="I15" s="30">
-        <v>15.5</v>
-      </c>
-      <c r="J15" s="30">
-        <v>15.5</v>
-      </c>
-      <c r="K15" s="30">
-        <v>15.5</v>
-      </c>
-      <c r="M15" s="27"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="32"/>
-      <c r="W15" s="15"/>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="32"/>
-      <c r="V16" s="32"/>
-      <c r="W16" s="15"/>
-    </row>
-    <row r="17" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="37"/>
-      <c r="C17" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="39">
-        <v>1</v>
-      </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
-      <c r="R17" s="43"/>
-      <c r="S17" s="43"/>
-      <c r="T17" s="43"/>
-      <c r="U17" s="43"/>
-      <c r="V17" s="43"/>
-      <c r="W17" s="15"/>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="43"/>
-      <c r="R18" s="43"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="43"/>
-      <c r="U18" s="43"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="15"/>
-    </row>
-    <row r="19" spans="2:23" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="49"/>
-      <c r="C19" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="52">
-        <f t="shared" ref="E19:K19" si="0">$D$17*E15</f>
-        <v>13.5</v>
-      </c>
-      <c r="F19" s="52">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G19" s="52">
-        <f t="shared" si="0"/>
-        <v>15.5</v>
-      </c>
-      <c r="H19" s="52">
-        <f t="shared" si="0"/>
-        <v>15.5</v>
-      </c>
-      <c r="I19" s="52">
-        <f t="shared" si="0"/>
-        <v>15.5</v>
-      </c>
-      <c r="J19" s="52">
-        <f t="shared" si="0"/>
-        <v>15.5</v>
-      </c>
-      <c r="K19" s="52">
-        <f t="shared" si="0"/>
-        <v>15.5</v>
-      </c>
-      <c r="M19" s="49"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="32"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="32"/>
-      <c r="W19" s="54"/>
-    </row>
-    <row r="20" spans="2:23" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="49"/>
-      <c r="C20" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="56"/>
-      <c r="E20" s="57">
-        <v>25</v>
-      </c>
-      <c r="F20" s="57">
-        <v>25</v>
-      </c>
-      <c r="G20" s="57">
-        <v>25</v>
-      </c>
-      <c r="H20" s="57">
-        <v>25</v>
-      </c>
-      <c r="I20" s="57">
-        <v>25</v>
-      </c>
-      <c r="J20" s="57">
-        <v>25</v>
-      </c>
-      <c r="K20" s="57">
-        <v>25</v>
-      </c>
-      <c r="M20" s="49"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="54"/>
-    </row>
-    <row r="21" spans="2:23" s="63" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="59"/>
-      <c r="C21" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="62">
-        <f>E20+E19</f>
-        <v>38.5</v>
-      </c>
-      <c r="F21" s="62">
-        <f t="shared" ref="F21:K21" si="1">F20+F19</f>
-        <v>34</v>
-      </c>
-      <c r="G21" s="62">
-        <f t="shared" si="1"/>
-        <v>40.5</v>
-      </c>
-      <c r="H21" s="62">
-        <f t="shared" si="1"/>
-        <v>40.5</v>
-      </c>
-      <c r="I21" s="62">
-        <f t="shared" si="1"/>
-        <v>40.5</v>
-      </c>
-      <c r="J21" s="62">
-        <f t="shared" si="1"/>
-        <v>40.5</v>
-      </c>
-      <c r="K21" s="62">
-        <f t="shared" si="1"/>
-        <v>40.5</v>
-      </c>
-      <c r="M21" s="59"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="65"/>
-      <c r="P21" s="66"/>
-      <c r="Q21" s="66"/>
-      <c r="R21" s="66"/>
-      <c r="S21" s="66"/>
-      <c r="T21" s="66"/>
-      <c r="U21" s="66"/>
-      <c r="V21" s="66"/>
-      <c r="W21" s="67"/>
-    </row>
-    <row r="22" spans="2:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="69"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="69"/>
-      <c r="S22" s="69"/>
-      <c r="T22" s="69"/>
-      <c r="U22" s="69"/>
-      <c r="V22" s="69"/>
-      <c r="W22" s="15"/>
-    </row>
-    <row r="23" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="71"/>
-      <c r="N23" s="70"/>
-      <c r="O23" s="70"/>
-      <c r="P23" s="71"/>
-      <c r="Q23" s="71"/>
-      <c r="R23" s="71"/>
-      <c r="S23" s="71"/>
-      <c r="T23" s="71"/>
-      <c r="U23" s="71"/>
-      <c r="V23" s="71"/>
-      <c r="W23" s="15"/>
-    </row>
-    <row r="24" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="71"/>
-      <c r="N24" s="70"/>
-      <c r="O24" s="70"/>
-      <c r="P24" s="71"/>
-      <c r="Q24" s="71"/>
-      <c r="R24" s="71"/>
-      <c r="S24" s="71"/>
-      <c r="T24" s="71"/>
-      <c r="U24" s="71"/>
-      <c r="V24" s="71"/>
-      <c r="W24" s="15"/>
-    </row>
-    <row r="25" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71"/>
-      <c r="K25" s="71"/>
-      <c r="N25" s="70"/>
-      <c r="O25" s="70"/>
-      <c r="P25" s="71"/>
-      <c r="Q25" s="71"/>
-      <c r="R25" s="71"/>
-      <c r="S25" s="71"/>
-      <c r="T25" s="71"/>
-      <c r="U25" s="71"/>
-      <c r="V25" s="71"/>
-      <c r="W25" s="15"/>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="72"/>
-      <c r="K27" s="72"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
-    </row>
-    <row r="28" spans="2:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="C28" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="73"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="75"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="76"/>
-      <c r="P28" s="77"/>
-      <c r="Q28" s="77"/>
-      <c r="R28" s="77"/>
-      <c r="S28" s="77"/>
-      <c r="T28" s="77"/>
-      <c r="U28" s="77"/>
-      <c r="V28" s="77"/>
-      <c r="W28" s="15"/>
-    </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B29" s="14"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="81"/>
-      <c r="J29" s="81"/>
-      <c r="K29" s="82"/>
-      <c r="N29" s="83"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="84"/>
-      <c r="R29" s="84"/>
-      <c r="S29" s="84"/>
-      <c r="T29" s="84"/>
-      <c r="U29" s="84"/>
-      <c r="V29" s="84"/>
-      <c r="W29" s="15"/>
-    </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B30" s="36"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="J30" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="K30" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="N30" s="25"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="26"/>
-      <c r="T30" s="26"/>
-      <c r="U30" s="26"/>
-      <c r="V30" s="26"/>
-      <c r="W30" s="15"/>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B31" s="27"/>
-      <c r="C31" s="28" t="str">
+      <c r="N30" s="17"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="18"/>
+      <c r="V30" s="18"/>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B31" s="19"/>
+      <c r="C31" s="81" t="str">
         <f>C15</f>
         <v>Hourly Rate</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="85">
-        <v>27</v>
-      </c>
-      <c r="F31" s="85">
-        <v>18</v>
-      </c>
-      <c r="G31" s="85">
-        <v>31</v>
-      </c>
-      <c r="H31" s="85">
-        <v>31</v>
-      </c>
-      <c r="I31" s="85">
-        <v>31</v>
-      </c>
-      <c r="J31" s="85">
-        <v>31</v>
-      </c>
-      <c r="K31" s="85">
-        <v>31</v>
-      </c>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="32"/>
-      <c r="R31" s="32"/>
-      <c r="S31" s="32"/>
-      <c r="T31" s="32"/>
-      <c r="U31" s="32"/>
-      <c r="V31" s="32"/>
-      <c r="W31" s="15"/>
-    </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B32" s="34"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="55">
+        <v>34</v>
+      </c>
+      <c r="F31" s="55">
+        <v>34</v>
+      </c>
+      <c r="G31" s="55">
+        <v>34</v>
+      </c>
+      <c r="H31" s="55">
+        <v>34</v>
+      </c>
+      <c r="I31" s="55">
+        <v>34</v>
+      </c>
+      <c r="J31" s="55">
+        <v>30</v>
+      </c>
+      <c r="N31" s="83"/>
+      <c r="O31" s="83"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B32" s="19"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
       <c r="N32" s="14"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="32"/>
-      <c r="R32" s="32"/>
-      <c r="S32" s="32"/>
-      <c r="T32" s="32"/>
-      <c r="U32" s="32"/>
-      <c r="V32" s="32"/>
-      <c r="W32" s="15"/>
-    </row>
-    <row r="33" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="34"/>
-      <c r="C33" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="39">
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+    </row>
+    <row r="33" spans="2:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="19"/>
+      <c r="C33" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="68">
         <v>1</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40"/>
-      <c r="N33" s="41"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="43"/>
-      <c r="Q33" s="43"/>
-      <c r="R33" s="43"/>
-      <c r="S33" s="43"/>
-      <c r="T33" s="43"/>
-      <c r="U33" s="43"/>
-      <c r="V33" s="43"/>
-      <c r="W33" s="15"/>
-    </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34" s="34"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="48"/>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="43"/>
-      <c r="R34" s="43"/>
-      <c r="S34" s="43"/>
-      <c r="T34" s="43"/>
-      <c r="U34" s="43"/>
-      <c r="V34" s="43"/>
-      <c r="W34" s="15"/>
-    </row>
-    <row r="35" spans="2:23" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="34"/>
-      <c r="C35" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="51"/>
-      <c r="E35" s="52">
-        <f t="shared" ref="E35:K35" si="2">$D$33*E31</f>
+      <c r="E33" s="84">
+        <f>ROUNDUP((2+($D33*$D34*140)/60),0)</f>
+        <v>5</v>
+      </c>
+      <c r="F33" s="86" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="72"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="24"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="24"/>
+    </row>
+    <row r="34" spans="2:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="19"/>
+      <c r="C34" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="71">
+        <v>1</v>
+      </c>
+      <c r="E34" s="85"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
+      <c r="T34" s="24"/>
+      <c r="U34" s="24"/>
+      <c r="V34" s="24"/>
+    </row>
+    <row r="35" spans="2:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="19"/>
+      <c r="C35" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="71">
+        <v>0</v>
+      </c>
+      <c r="E35" s="77">
+        <f>ROUNDUP((($D35*40)/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="24"/>
+      <c r="T35" s="24"/>
+      <c r="U35" s="24"/>
+      <c r="V35" s="24"/>
+    </row>
+    <row r="36" spans="2:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="19"/>
+      <c r="C36" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="71">
+        <v>0</v>
+      </c>
+      <c r="E36" s="77">
+        <f>ROUNDUP((($D36*70)/60),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="T36" s="24"/>
+      <c r="U36" s="24"/>
+      <c r="V36" s="24"/>
+    </row>
+    <row r="37" spans="2:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="19"/>
+      <c r="C37" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="F35" s="52">
+      <c r="D37" s="75">
+        <f>D33*D34+D35+D36</f>
+        <v>1</v>
+      </c>
+      <c r="E37" s="73">
+        <f>SUM(E33:E36)</f>
+        <v>5</v>
+      </c>
+      <c r="F37" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="25"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="24"/>
+      <c r="T37" s="24"/>
+      <c r="U37" s="24"/>
+      <c r="V37" s="24"/>
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B38" s="19"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="30"/>
+      <c r="P38" s="24"/>
+      <c r="Q38" s="24"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="24"/>
+      <c r="T38" s="24"/>
+      <c r="U38" s="24"/>
+      <c r="V38" s="24"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B39" s="19"/>
+      <c r="C39" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="32"/>
+      <c r="E39" s="33">
+        <f>$E$37*E31</f>
+        <v>170</v>
+      </c>
+      <c r="F39" s="33">
+        <f t="shared" ref="F39:J39" si="2">$E$37*F31</f>
+        <v>170</v>
+      </c>
+      <c r="G39" s="33">
         <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="G35" s="52">
+        <v>170</v>
+      </c>
+      <c r="H39" s="33">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="H35" s="52">
+        <v>170</v>
+      </c>
+      <c r="I39" s="33">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="I35" s="52">
+        <v>170</v>
+      </c>
+      <c r="J39" s="33">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="J35" s="52">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="K35" s="52">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="N35" s="36"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="32"/>
-      <c r="Q35" s="32"/>
-      <c r="R35" s="32"/>
-      <c r="S35" s="32"/>
-      <c r="T35" s="32"/>
-      <c r="U35" s="32"/>
-      <c r="V35" s="32"/>
-      <c r="W35" s="54"/>
-    </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B36" s="34"/>
-      <c r="C36" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="56"/>
-      <c r="E36" s="57">
-        <v>25</v>
-      </c>
-      <c r="F36" s="57">
-        <v>25</v>
-      </c>
-      <c r="G36" s="57">
-        <v>25</v>
-      </c>
-      <c r="H36" s="57">
-        <v>25</v>
-      </c>
-      <c r="I36" s="57">
-        <v>25</v>
-      </c>
-      <c r="J36" s="57">
-        <v>25</v>
-      </c>
-      <c r="K36" s="57">
-        <v>25</v>
-      </c>
-      <c r="N36" s="36"/>
-      <c r="O36" s="58"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="32"/>
-      <c r="R36" s="32"/>
-      <c r="S36" s="32"/>
-      <c r="T36" s="32"/>
-      <c r="U36" s="32"/>
-      <c r="V36" s="32"/>
-      <c r="W36" s="15"/>
-    </row>
-    <row r="37" spans="2:23" s="63" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="86"/>
-      <c r="C37" s="60" t="str">
-        <f>C21</f>
-        <v>Total Cost:</v>
-      </c>
-      <c r="D37" s="61"/>
-      <c r="E37" s="62">
-        <f>E36+E35</f>
-        <v>52</v>
-      </c>
-      <c r="F37" s="62">
-        <f t="shared" ref="F37:K37" si="3">F36+F35</f>
-        <v>43</v>
-      </c>
-      <c r="G37" s="62">
-        <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="H37" s="62">
-        <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="I37" s="62">
-        <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="J37" s="62">
-        <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="K37" s="62">
-        <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="N37" s="64"/>
-      <c r="O37" s="65"/>
-      <c r="P37" s="66"/>
-      <c r="Q37" s="66"/>
-      <c r="R37" s="66"/>
-      <c r="S37" s="66"/>
-      <c r="T37" s="66"/>
-      <c r="U37" s="66"/>
-      <c r="V37" s="66"/>
-      <c r="W37" s="67"/>
-    </row>
-    <row r="38" spans="2:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="34"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="87"/>
-      <c r="J38" s="87"/>
-      <c r="K38" s="87"/>
-      <c r="N38" s="36"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="88"/>
-      <c r="Q38" s="88"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="88"/>
-      <c r="U38" s="88"/>
-      <c r="V38" s="88"/>
-      <c r="W38" s="15"/>
-    </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39" s="34"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="87"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="87"/>
-      <c r="H39" s="87"/>
-      <c r="I39" s="87"/>
-      <c r="J39" s="87"/>
-      <c r="K39" s="87"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
-      <c r="U39" s="15"/>
-      <c r="V39" s="15"/>
-      <c r="W39" s="15"/>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B40" s="34"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="87"/>
-      <c r="F40" s="87"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="87"/>
-      <c r="I40" s="87"/>
-      <c r="J40" s="87"/>
-      <c r="K40" s="87"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="15"/>
-      <c r="U40" s="15"/>
-      <c r="V40" s="15"/>
-      <c r="W40" s="15"/>
-    </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41" s="34"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="87"/>
-      <c r="F41" s="87"/>
-      <c r="G41" s="87"/>
-      <c r="H41" s="87"/>
-      <c r="I41" s="87"/>
-      <c r="J41" s="87"/>
-      <c r="K41" s="87"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
-      <c r="U41" s="15"/>
-      <c r="V41" s="15"/>
-      <c r="W41" s="15"/>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B42" s="34"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="87"/>
-      <c r="F42" s="87"/>
-      <c r="G42" s="87"/>
-      <c r="H42" s="87"/>
-      <c r="I42" s="87"/>
-      <c r="J42" s="87"/>
-      <c r="K42" s="87"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
-      <c r="T42" s="15"/>
-      <c r="U42" s="15"/>
-      <c r="V42" s="15"/>
-      <c r="W42" s="15"/>
-    </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B43" s="34"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="87"/>
-      <c r="F43" s="87"/>
-      <c r="G43" s="87"/>
-      <c r="H43" s="87"/>
-      <c r="I43" s="87"/>
-      <c r="J43" s="87"/>
-      <c r="K43" s="87"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
-    </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B44" s="34"/>
+        <v>150</v>
+      </c>
+      <c r="N39" s="22"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="21"/>
+      <c r="V39" s="21"/>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B40" s="19"/>
+      <c r="C40" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="35"/>
+      <c r="E40" s="36">
+        <v>27</v>
+      </c>
+      <c r="F40" s="36">
+        <v>27</v>
+      </c>
+      <c r="G40" s="36">
+        <v>27</v>
+      </c>
+      <c r="H40" s="36">
+        <v>27</v>
+      </c>
+      <c r="I40" s="36">
+        <v>27</v>
+      </c>
+      <c r="J40" s="36">
+        <v>27</v>
+      </c>
+      <c r="N40" s="22"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="21"/>
+    </row>
+    <row r="41" spans="2:22" s="41" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="56"/>
+      <c r="C41" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="39"/>
+      <c r="E41" s="40">
+        <f t="shared" ref="E41" si="3">E40+E39</f>
+        <v>197</v>
+      </c>
+      <c r="F41" s="40">
+        <f>F40+F39</f>
+        <v>197</v>
+      </c>
+      <c r="G41" s="40">
+        <f>G40+G39</f>
+        <v>197</v>
+      </c>
+      <c r="H41" s="40">
+        <f>H40+H39</f>
+        <v>197</v>
+      </c>
+      <c r="I41" s="40">
+        <f>I40+I39</f>
+        <v>197</v>
+      </c>
+      <c r="J41" s="40">
+        <f>J40+J39</f>
+        <v>177</v>
+      </c>
+      <c r="N41" s="42"/>
+      <c r="O41" s="43"/>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="44"/>
+      <c r="R41" s="44"/>
+      <c r="S41" s="44"/>
+      <c r="T41" s="44"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="44"/>
+    </row>
+    <row r="42" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="19"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="57"/>
+      <c r="K42" s="57"/>
+      <c r="N42" s="22"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="57"/>
+      <c r="Q42" s="57"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="57"/>
+      <c r="U42" s="57"/>
+      <c r="V42" s="57"/>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B43" s="19"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="57"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B44" s="19"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
+      <c r="K44" s="57"/>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B45" s="19"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="57"/>
+      <c r="K45" s="57"/>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B46" s="19"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+    </row>
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B47" s="19"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+    </row>
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B48" s="19"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="D17 D33 O17 O33" name="Range1"/>
+    <protectedRange sqref="D17 E37 O17 O33:O37 D33:D36" name="Range1"/>
   </protectedRanges>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="N31:O31"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J10" r:id="rId1" display="for a detailed description check out our website resources page"/>
+    <hyperlink ref="J8" r:id="rId1" display="for a detailed description check out our website resources page" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>